<commit_message>
freq entropy results fixed
</commit_message>
<xml_diff>
--- a/output_ex/param_results.xlsx
+++ b/output_ex/param_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pelin/projects/github_release/recentvschronic/output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pelin/projects/github_release/recentvschronic/output_ex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353F0197-90EC-664E-B926-D405E4401917}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4CFAA8-0C4F-024A-B793-E2DACC4978A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25400" yWindow="460" windowWidth="27640" windowHeight="14900" activeTab="1" xr2:uid="{4BB309F5-563A-9045-B150-C7190C524EC1}"/>
+    <workbookView xWindow="-25600" yWindow="460" windowWidth="25600" windowHeight="13920" xr2:uid="{4BB309F5-563A-9045-B150-C7190C524EC1}"/>
   </bookViews>
   <sheets>
     <sheet name="16Params" sheetId="1" r:id="rId1"/>
@@ -454,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D3DD46-4069-0E49-8987-84A06D114EB7}">
   <dimension ref="A1:Q355"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:Q355"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -613,7 +613,7 @@
         <v>0.58439099999999999</v>
       </c>
       <c r="N3">
-        <v>0.84084150627241505</v>
+        <v>0.71424675440524299</v>
       </c>
       <c r="O3">
         <v>-1</v>
@@ -666,7 +666,7 @@
         <v>0.443326</v>
       </c>
       <c r="N4">
-        <v>0.84084150627241505</v>
+        <v>0.80095261891591696</v>
       </c>
       <c r="O4">
         <v>-1</v>
@@ -719,7 +719,7 @@
         <v>0.39080799999999999</v>
       </c>
       <c r="N5">
-        <v>0.84084150627241505</v>
+        <v>0.74231537994317698</v>
       </c>
       <c r="O5">
         <v>-1</v>
@@ -772,7 +772,7 @@
         <v>0.31675700000000001</v>
       </c>
       <c r="N6">
-        <v>0.84084150627241505</v>
+        <v>0.75653964109816196</v>
       </c>
       <c r="O6">
         <v>-1</v>
@@ -825,7 +825,7 @@
         <v>0.85434399999999999</v>
       </c>
       <c r="N7">
-        <v>0.84084150627241505</v>
+        <v>0.83440956031939395</v>
       </c>
       <c r="O7">
         <v>-1</v>
@@ -878,7 +878,7 @@
         <v>0.446602</v>
       </c>
       <c r="N8">
-        <v>0.84084150627241505</v>
+        <v>0.69670829601186002</v>
       </c>
       <c r="O8">
         <v>-1</v>
@@ -931,7 +931,7 @@
         <v>0.70462000000000002</v>
       </c>
       <c r="N9">
-        <v>0.84084150627241505</v>
+        <v>0.85138686946495401</v>
       </c>
       <c r="O9">
         <v>-1</v>
@@ -984,7 +984,7 @@
         <v>0.45526499999999998</v>
       </c>
       <c r="N10">
-        <v>0.84084150627241505</v>
+        <v>0.78438310878128703</v>
       </c>
       <c r="O10">
         <v>-1</v>
@@ -1037,7 +1037,7 @@
         <v>0.56062500000000004</v>
       </c>
       <c r="N11">
-        <v>0.84084150627241505</v>
+        <v>0.70440017659356702</v>
       </c>
       <c r="O11">
         <v>-1</v>
@@ -1090,7 +1090,7 @@
         <v>0.83331299999999997</v>
       </c>
       <c r="N12">
-        <v>0.84084150627241505</v>
+        <v>0.91617459763546205</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -1143,7 +1143,7 @@
         <v>0.39104299999999997</v>
       </c>
       <c r="N13">
-        <v>0.84084150627241505</v>
+        <v>0.77504194531915105</v>
       </c>
       <c r="O13">
         <v>-1</v>
@@ -1196,7 +1196,7 @@
         <v>0.52660300000000004</v>
       </c>
       <c r="N14">
-        <v>0.84084150627241505</v>
+        <v>0.82098972265952797</v>
       </c>
       <c r="O14">
         <v>-1</v>
@@ -1249,7 +1249,7 @@
         <v>0.846248</v>
       </c>
       <c r="N15">
-        <v>0.84084150627241505</v>
+        <v>0.863280979127657</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -1302,7 +1302,7 @@
         <v>0.86460000000000004</v>
       </c>
       <c r="N16">
-        <v>0.84084150627241505</v>
+        <v>0.90493097104845999</v>
       </c>
       <c r="O16">
         <v>-1</v>
@@ -1355,7 +1355,7 @@
         <v>0.56034200000000001</v>
       </c>
       <c r="N17">
-        <v>0.84084150627241505</v>
+        <v>0.81417478004714605</v>
       </c>
       <c r="O17">
         <v>-1</v>
@@ -1408,7 +1408,7 @@
         <v>0.74745799999999996</v>
       </c>
       <c r="N18">
-        <v>0.84084150627241505</v>
+        <v>0.79538491548711399</v>
       </c>
       <c r="O18">
         <v>-1</v>
@@ -1461,7 +1461,7 @@
         <v>0.337922</v>
       </c>
       <c r="N19">
-        <v>0.84084150627241505</v>
+        <v>0.76958622165233503</v>
       </c>
       <c r="O19">
         <v>-1</v>
@@ -1514,7 +1514,7 @@
         <v>0.44853500000000002</v>
       </c>
       <c r="N20">
-        <v>0.84084150627241505</v>
+        <v>0.76581411334910898</v>
       </c>
       <c r="O20">
         <v>-1</v>
@@ -1567,7 +1567,7 @@
         <v>0.37603199999999998</v>
       </c>
       <c r="N21">
-        <v>0.84084150627241505</v>
+        <v>0.569727836339052</v>
       </c>
       <c r="O21">
         <v>1</v>
@@ -1620,7 +1620,7 @@
         <v>0.821793</v>
       </c>
       <c r="N22">
-        <v>0.84084150627241505</v>
+        <v>0.78481260374550599</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -1673,7 +1673,7 @@
         <v>1.0021929999999999</v>
       </c>
       <c r="N23">
-        <v>0.84084150627241505</v>
+        <v>0.81811832464399303</v>
       </c>
       <c r="O23">
         <v>-1</v>
@@ -1726,7 +1726,7 @@
         <v>0.61360899999999996</v>
       </c>
       <c r="N24">
-        <v>0.84084150627241505</v>
+        <v>0.79876080288356299</v>
       </c>
       <c r="O24">
         <v>-1</v>
@@ -1779,7 +1779,7 @@
         <v>0.71816000000000002</v>
       </c>
       <c r="N25">
-        <v>0.84084150627241505</v>
+        <v>0.68737634698245598</v>
       </c>
       <c r="O25">
         <v>-1</v>
@@ -1832,7 +1832,7 @@
         <v>0.44482100000000002</v>
       </c>
       <c r="N26">
-        <v>0.84084150627241505</v>
+        <v>0.49524652706820499</v>
       </c>
       <c r="O26">
         <v>1</v>
@@ -1885,7 +1885,7 @@
         <v>0.62227699999999997</v>
       </c>
       <c r="N27">
-        <v>0.84084150627241505</v>
+        <v>0.66501869440745898</v>
       </c>
       <c r="O27">
         <v>-1</v>
@@ -1938,7 +1938,7 @@
         <v>1.1079559999999999</v>
       </c>
       <c r="N28">
-        <v>0.84084150627241505</v>
+        <v>0.81969389493410105</v>
       </c>
       <c r="O28">
         <v>-1</v>
@@ -1991,7 +1991,7 @@
         <v>0.70469099999999996</v>
       </c>
       <c r="N29">
-        <v>0.84084150627241505</v>
+        <v>0.69667747349140996</v>
       </c>
       <c r="O29">
         <v>-1</v>
@@ -2044,7 +2044,7 @@
         <v>0.86250499999999997</v>
       </c>
       <c r="N30">
-        <v>0.84084150627241505</v>
+        <v>0.77500450321488501</v>
       </c>
       <c r="O30">
         <v>-1</v>
@@ -2097,7 +2097,7 @@
         <v>0.58136100000000002</v>
       </c>
       <c r="N31">
-        <v>0.84084150627241505</v>
+        <v>0.43800737135560702</v>
       </c>
       <c r="O31">
         <v>1</v>
@@ -2150,7 +2150,7 @@
         <v>0.43767600000000001</v>
       </c>
       <c r="N32">
-        <v>0.84084150627241505</v>
+        <v>0.61748988424528095</v>
       </c>
       <c r="O32">
         <v>1</v>
@@ -2203,7 +2203,7 @@
         <v>0.55891800000000003</v>
       </c>
       <c r="N33">
-        <v>0.84084150627241505</v>
+        <v>0.48853732029279201</v>
       </c>
       <c r="O33">
         <v>1</v>
@@ -2256,7 +2256,7 @@
         <v>0.67210599999999998</v>
       </c>
       <c r="N34">
-        <v>0.84084150627241505</v>
+        <v>0.57610906113391003</v>
       </c>
       <c r="O34">
         <v>1</v>
@@ -2309,7 +2309,7 @@
         <v>0.56631900000000002</v>
       </c>
       <c r="N35">
-        <v>0.84084150627241505</v>
+        <v>0.79892485350397102</v>
       </c>
       <c r="O35">
         <v>-1</v>
@@ -2362,7 +2362,7 @@
         <v>0.57774000000000003</v>
       </c>
       <c r="N36">
-        <v>0.84084150627241505</v>
+        <v>0.77894854764530097</v>
       </c>
       <c r="O36">
         <v>-1</v>
@@ -2415,7 +2415,7 @@
         <v>0.55593800000000004</v>
       </c>
       <c r="N37">
-        <v>0.84084150627241505</v>
+        <v>0.57730592451187102</v>
       </c>
       <c r="O37">
         <v>-1</v>
@@ -2468,7 +2468,7 @@
         <v>0.87194300000000002</v>
       </c>
       <c r="N38">
-        <v>0.84084150627241505</v>
+        <v>0.87981522720224803</v>
       </c>
       <c r="O38">
         <v>-1</v>
@@ -2521,7 +2521,7 @@
         <v>0.56063799999999997</v>
       </c>
       <c r="N39">
-        <v>0.84084150627241505</v>
+        <v>0.59584587965033597</v>
       </c>
       <c r="O39">
         <v>1</v>
@@ -2574,7 +2574,7 @@
         <v>0.83472100000000005</v>
       </c>
       <c r="N40">
-        <v>0.84084150627241505</v>
+        <v>0.66726895273829101</v>
       </c>
       <c r="O40">
         <v>-1</v>
@@ -2627,7 +2627,7 @@
         <v>0.89827100000000004</v>
       </c>
       <c r="N41">
-        <v>0.84084150627241505</v>
+        <v>0.69441877887052605</v>
       </c>
       <c r="O41">
         <v>-1</v>
@@ -2680,7 +2680,7 @@
         <v>0.95708000000000004</v>
       </c>
       <c r="N42">
-        <v>0.84084150627241505</v>
+        <v>0.69643459274178998</v>
       </c>
       <c r="O42">
         <v>-1</v>
@@ -2733,7 +2733,7 @@
         <v>0.66555600000000004</v>
       </c>
       <c r="N43">
-        <v>0.84084150627241505</v>
+        <v>0.85867023112465801</v>
       </c>
       <c r="O43">
         <v>-1</v>
@@ -2786,7 +2786,7 @@
         <v>0.84455599999999997</v>
       </c>
       <c r="N44">
-        <v>0.84084150627241505</v>
+        <v>0.84136147028128705</v>
       </c>
       <c r="O44">
         <v>-1</v>
@@ -2839,7 +2839,7 @@
         <v>1.1687069999999999</v>
       </c>
       <c r="N45">
-        <v>0.84084150627241505</v>
+        <v>0.70258990867011695</v>
       </c>
       <c r="O45">
         <v>-1</v>
@@ -2892,7 +2892,7 @@
         <v>0.97773699999999997</v>
       </c>
       <c r="N46">
-        <v>0.84084150627241505</v>
+        <v>0.87573134367049799</v>
       </c>
       <c r="O46">
         <v>0</v>
@@ -2945,7 +2945,7 @@
         <v>0.80173700000000003</v>
       </c>
       <c r="N47">
-        <v>0.84084150627241505</v>
+        <v>0.81563424722065903</v>
       </c>
       <c r="O47">
         <v>-1</v>
@@ -2998,7 +2998,7 @@
         <v>0.79407700000000003</v>
       </c>
       <c r="N48">
-        <v>0.84084150627241505</v>
+        <v>0.67198370681909902</v>
       </c>
       <c r="O48">
         <v>-1</v>
@@ -3051,7 +3051,7 @@
         <v>0.88898999999999995</v>
       </c>
       <c r="N49">
-        <v>0.84084150627241505</v>
+        <v>0.83408889958589805</v>
       </c>
       <c r="O49">
         <v>-1</v>
@@ -3104,7 +3104,7 @@
         <v>0.97412100000000001</v>
       </c>
       <c r="N50">
-        <v>0.84084150627241505</v>
+        <v>0.71476210159532505</v>
       </c>
       <c r="O50">
         <v>0</v>
@@ -3157,7 +3157,7 @@
         <v>0.93194500000000002</v>
       </c>
       <c r="N51">
-        <v>0.84084150627241505</v>
+        <v>0.753928144260679</v>
       </c>
       <c r="O51">
         <v>-1</v>
@@ -3210,7 +3210,7 @@
         <v>0.55153700000000005</v>
       </c>
       <c r="N52">
-        <v>0.84084150627241505</v>
+        <v>0.365707065332254</v>
       </c>
       <c r="O52">
         <v>1</v>
@@ -3263,7 +3263,7 @@
         <v>0.97058800000000001</v>
       </c>
       <c r="N53">
-        <v>0.84084150627241505</v>
+        <v>0.86434967126515705</v>
       </c>
       <c r="O53">
         <v>-1</v>
@@ -3316,7 +3316,7 @@
         <v>0.58828199999999997</v>
       </c>
       <c r="N54">
-        <v>0.84084150627241505</v>
+        <v>0.77389280659890702</v>
       </c>
       <c r="O54">
         <v>-1</v>
@@ -3369,7 +3369,7 @@
         <v>0.750417</v>
       </c>
       <c r="N55">
-        <v>0.84084150627241505</v>
+        <v>0.71744204358527996</v>
       </c>
       <c r="O55">
         <v>0</v>
@@ -3422,7 +3422,7 @@
         <v>0.81240400000000002</v>
       </c>
       <c r="N56">
-        <v>0.84084150627241505</v>
+        <v>0.87439285629226404</v>
       </c>
       <c r="O56">
         <v>-1</v>
@@ -3475,7 +3475,7 @@
         <v>0.37121500000000002</v>
       </c>
       <c r="N57">
-        <v>0.84084150627241505</v>
+        <v>0.467657770243111</v>
       </c>
       <c r="O57">
         <v>1</v>
@@ -3528,7 +3528,7 @@
         <v>0.78873000000000004</v>
       </c>
       <c r="N58">
-        <v>0.84084150627241505</v>
+        <v>0.80898927933059905</v>
       </c>
       <c r="O58">
         <v>-1</v>
@@ -3581,7 +3581,7 @@
         <v>0.65490899999999996</v>
       </c>
       <c r="N59">
-        <v>0.84084150627241505</v>
+        <v>0.85393679270921996</v>
       </c>
       <c r="O59">
         <v>0</v>
@@ -3634,7 +3634,7 @@
         <v>0.74248800000000004</v>
       </c>
       <c r="N60">
-        <v>0.84084150627241505</v>
+        <v>0.91664578812965503</v>
       </c>
       <c r="O60">
         <v>-1</v>
@@ -3687,7 +3687,7 @@
         <v>0.55786599999999997</v>
       </c>
       <c r="N61">
-        <v>0.84084150627241505</v>
+        <v>0.60468840690605197</v>
       </c>
       <c r="O61">
         <v>0</v>
@@ -3740,7 +3740,7 @@
         <v>0.54949499999999996</v>
       </c>
       <c r="N62">
-        <v>0.84084150627241505</v>
+        <v>0.88441871153083296</v>
       </c>
       <c r="O62">
         <v>0</v>
@@ -3793,7 +3793,7 @@
         <v>0.55718500000000004</v>
       </c>
       <c r="N63">
-        <v>0.84084150627241505</v>
+        <v>0.63767904194540503</v>
       </c>
       <c r="O63">
         <v>-1</v>
@@ -3846,7 +3846,7 @@
         <v>0.35399799999999998</v>
       </c>
       <c r="N64">
-        <v>0.84084150627241505</v>
+        <v>0.44755828647057999</v>
       </c>
       <c r="O64">
         <v>1</v>
@@ -3899,7 +3899,7 @@
         <v>0.46854499999999999</v>
       </c>
       <c r="N65">
-        <v>0.84084150627241505</v>
+        <v>0.49765902039472598</v>
       </c>
       <c r="O65">
         <v>-1</v>
@@ -3952,7 +3952,7 @@
         <v>0.69069899999999995</v>
       </c>
       <c r="N66">
-        <v>0.84084150627241505</v>
+        <v>0.59276438060712799</v>
       </c>
       <c r="O66">
         <v>1</v>
@@ -4005,7 +4005,7 @@
         <v>0.57105600000000001</v>
       </c>
       <c r="N67">
-        <v>0.84084150627241505</v>
+        <v>0.46404578099302801</v>
       </c>
       <c r="O67">
         <v>-1</v>
@@ -4058,7 +4058,7 @@
         <v>0.75669200000000003</v>
       </c>
       <c r="N68">
-        <v>0.84084150627241505</v>
+        <v>0.82266120503718898</v>
       </c>
       <c r="O68">
         <v>-1</v>
@@ -4111,7 +4111,7 @@
         <v>1.058487</v>
       </c>
       <c r="N69">
-        <v>0.84084150627241505</v>
+        <v>0.799357102066512</v>
       </c>
       <c r="O69">
         <v>-1</v>
@@ -4164,7 +4164,7 @@
         <v>0.91153899999999999</v>
       </c>
       <c r="N70">
-        <v>0.84084150627241505</v>
+        <v>0.41329397532698597</v>
       </c>
       <c r="O70">
         <v>-1</v>
@@ -4217,7 +4217,7 @@
         <v>0.43545899999999998</v>
       </c>
       <c r="N71">
-        <v>0.84084150627241505</v>
+        <v>0.29754159105044697</v>
       </c>
       <c r="O71">
         <v>1</v>
@@ -4270,7 +4270,7 @@
         <v>1.262232</v>
       </c>
       <c r="N72">
-        <v>0.84084150627241505</v>
+        <v>0.82529316235859695</v>
       </c>
       <c r="O72">
         <v>-1</v>
@@ -4323,7 +4323,7 @@
         <v>0.91847900000000005</v>
       </c>
       <c r="N73">
-        <v>0.84084150627241505</v>
+        <v>0.75840806846861197</v>
       </c>
       <c r="O73">
         <v>-1</v>
@@ -4376,7 +4376,7 @@
         <v>1.074001</v>
       </c>
       <c r="N74">
-        <v>0.84084150627241505</v>
+        <v>0.74481450888451395</v>
       </c>
       <c r="O74">
         <v>-1</v>
@@ -4429,7 +4429,7 @@
         <v>0.70589500000000005</v>
       </c>
       <c r="N75">
-        <v>0.84084150627241505</v>
+        <v>0.83722606971831803</v>
       </c>
       <c r="O75">
         <v>-1</v>
@@ -4482,7 +4482,7 @@
         <v>0.44808900000000002</v>
       </c>
       <c r="N76">
-        <v>0.84084150627241505</v>
+        <v>0.66194947945506699</v>
       </c>
       <c r="O76">
         <v>1</v>
@@ -4535,7 +4535,7 @@
         <v>0.365539</v>
       </c>
       <c r="N77">
-        <v>0.84084150627241505</v>
+        <v>0.277456682441376</v>
       </c>
       <c r="O77">
         <v>0</v>
@@ -4588,7 +4588,7 @@
         <v>1.100328</v>
       </c>
       <c r="N78">
-        <v>0.84084150627241505</v>
+        <v>0.93455409777991005</v>
       </c>
       <c r="O78">
         <v>-1</v>
@@ -4641,7 +4641,7 @@
         <v>0.49078699999999997</v>
       </c>
       <c r="N79">
-        <v>0.84084150627241505</v>
+        <v>0.34065319624514201</v>
       </c>
       <c r="O79">
         <v>1</v>
@@ -4694,7 +4694,7 @@
         <v>0.92191100000000004</v>
       </c>
       <c r="N80">
-        <v>0.84084150627241505</v>
+        <v>0.77498603840746505</v>
       </c>
       <c r="O80">
         <v>0</v>
@@ -4747,7 +4747,7 @@
         <v>0.37479299999999999</v>
       </c>
       <c r="N81">
-        <v>0.84084150627241505</v>
+        <v>0.63032245408530596</v>
       </c>
       <c r="O81">
         <v>1</v>
@@ -4800,7 +4800,7 @@
         <v>0.41345900000000002</v>
       </c>
       <c r="N82">
-        <v>0.84084150627241505</v>
+        <v>0.45332588241300997</v>
       </c>
       <c r="O82">
         <v>0</v>
@@ -4853,7 +4853,7 @@
         <v>0.53062200000000004</v>
       </c>
       <c r="N83">
-        <v>0.84084150627241505</v>
+        <v>0.75327173814747705</v>
       </c>
       <c r="O83">
         <v>0</v>
@@ -4906,7 +4906,7 @@
         <v>0.82101000000000002</v>
       </c>
       <c r="N84">
-        <v>0.84084150627241505</v>
+        <v>0.81191831932487801</v>
       </c>
       <c r="O84">
         <v>0</v>
@@ -4959,7 +4959,7 @@
         <v>0.827654</v>
       </c>
       <c r="N85">
-        <v>0.84084150627241505</v>
+        <v>0.69963099071847801</v>
       </c>
       <c r="O85">
         <v>1</v>
@@ -5012,7 +5012,7 @@
         <v>0.66126499999999999</v>
       </c>
       <c r="N86">
-        <v>0.84084150627241505</v>
+        <v>0.84095378919046404</v>
       </c>
       <c r="O86">
         <v>-1</v>
@@ -5065,7 +5065,7 @@
         <v>0.84989899999999996</v>
       </c>
       <c r="N87">
-        <v>0.84084150627241505</v>
+        <v>0.71935919889866196</v>
       </c>
       <c r="O87">
         <v>-1</v>
@@ -5118,7 +5118,7 @@
         <v>0.586588</v>
       </c>
       <c r="N88">
-        <v>0.84084150627241505</v>
+        <v>0.59765544927474001</v>
       </c>
       <c r="O88">
         <v>1</v>
@@ -5171,7 +5171,7 @@
         <v>1.1402570000000001</v>
       </c>
       <c r="N89">
-        <v>0.84084150627241505</v>
+        <v>0.81743658707606204</v>
       </c>
       <c r="O89">
         <v>-1</v>
@@ -5224,7 +5224,7 @@
         <v>0.84384700000000001</v>
       </c>
       <c r="N90">
-        <v>0.84084150627241505</v>
+        <v>0.82843186916919498</v>
       </c>
       <c r="O90">
         <v>-1</v>
@@ -5277,7 +5277,7 @@
         <v>0.49026500000000001</v>
       </c>
       <c r="N91">
-        <v>0.84084150627241505</v>
+        <v>0.48723904347626401</v>
       </c>
       <c r="O91">
         <v>1</v>
@@ -5330,7 +5330,7 @@
         <v>0.55756399999999995</v>
       </c>
       <c r="N92">
-        <v>0.84084150627241505</v>
+        <v>0.79134073176261899</v>
       </c>
       <c r="O92">
         <v>-1</v>
@@ -5383,7 +5383,7 @@
         <v>1.036797</v>
       </c>
       <c r="N93">
-        <v>0.84084150627241505</v>
+        <v>0.91519927885102104</v>
       </c>
       <c r="O93">
         <v>-1</v>
@@ -5436,7 +5436,7 @@
         <v>0.43820100000000001</v>
       </c>
       <c r="N94">
-        <v>0.84084150627241505</v>
+        <v>0.40107776582946503</v>
       </c>
       <c r="O94">
         <v>1</v>
@@ -5489,7 +5489,7 @@
         <v>0.54617800000000005</v>
       </c>
       <c r="N95">
-        <v>0.84084150627241505</v>
+        <v>0.753574969892985</v>
       </c>
       <c r="O95">
         <v>-1</v>
@@ -5542,7 +5542,7 @@
         <v>0.31223699999999999</v>
       </c>
       <c r="N96">
-        <v>0.84084150627241505</v>
+        <v>0.51319973395274598</v>
       </c>
       <c r="O96">
         <v>1</v>
@@ -5595,7 +5595,7 @@
         <v>0.398061</v>
       </c>
       <c r="N97">
-        <v>0.84084150627241505</v>
+        <v>0.475013974354274</v>
       </c>
       <c r="O97">
         <v>1</v>
@@ -5648,7 +5648,7 @@
         <v>0.97115799999999997</v>
       </c>
       <c r="N98">
-        <v>0.84084150627241505</v>
+        <v>0.817849726982251</v>
       </c>
       <c r="O98">
         <v>1</v>
@@ -5701,7 +5701,7 @@
         <v>0.54408699999999999</v>
       </c>
       <c r="N99">
-        <v>0.84084150627241505</v>
+        <v>0.83130700643641597</v>
       </c>
       <c r="O99">
         <v>-1</v>
@@ -5754,7 +5754,7 @@
         <v>0.33842299999999997</v>
       </c>
       <c r="N100">
-        <v>0.84084150627241505</v>
+        <v>0.48566641188374898</v>
       </c>
       <c r="O100">
         <v>1</v>
@@ -5807,7 +5807,7 @@
         <v>0.85845700000000003</v>
       </c>
       <c r="N101">
-        <v>0.84084150627241505</v>
+        <v>0.61788168098794305</v>
       </c>
       <c r="O101">
         <v>-1</v>
@@ -5860,7 +5860,7 @@
         <v>0.222857</v>
       </c>
       <c r="N102">
-        <v>0.84084150627241505</v>
+        <v>0.248208269733866</v>
       </c>
       <c r="O102">
         <v>0</v>
@@ -5913,7 +5913,7 @@
         <v>0.39459699999999998</v>
       </c>
       <c r="N103">
-        <v>0.84084150627241505</v>
+        <v>0.600624128065672</v>
       </c>
       <c r="O103">
         <v>-1</v>
@@ -5966,7 +5966,7 @@
         <v>0.64586200000000005</v>
       </c>
       <c r="N104">
-        <v>0.84084150627241505</v>
+        <v>0.69036971993581397</v>
       </c>
       <c r="O104">
         <v>-1</v>
@@ -6019,7 +6019,7 @@
         <v>0.43876199999999999</v>
       </c>
       <c r="N105">
-        <v>0.84084150627241505</v>
+        <v>0.60228219023915996</v>
       </c>
       <c r="O105">
         <v>1</v>
@@ -6072,7 +6072,7 @@
         <v>0.43970799999999999</v>
       </c>
       <c r="N106">
-        <v>0.84084150627241505</v>
+        <v>0.44437362038995998</v>
       </c>
       <c r="O106">
         <v>0</v>
@@ -6125,7 +6125,7 @@
         <v>0.75298200000000004</v>
       </c>
       <c r="N107">
-        <v>0.84084150627241505</v>
+        <v>0.58575540098051304</v>
       </c>
       <c r="O107">
         <v>0</v>
@@ -6178,7 +6178,7 @@
         <v>0.55852900000000005</v>
       </c>
       <c r="N108">
-        <v>0.84084150627241505</v>
+        <v>0.68065381639218103</v>
       </c>
       <c r="O108">
         <v>0</v>
@@ -6231,7 +6231,7 @@
         <v>0.31689400000000001</v>
       </c>
       <c r="N109">
-        <v>0.84084150627241505</v>
+        <v>0.60465764346391904</v>
       </c>
       <c r="O109">
         <v>0</v>
@@ -6284,7 +6284,7 @@
         <v>0.59237399999999996</v>
       </c>
       <c r="N110">
-        <v>0.84084150627241505</v>
+        <v>0.55691661353290001</v>
       </c>
       <c r="O110">
         <v>1</v>
@@ -6337,7 +6337,7 @@
         <v>0.96356900000000001</v>
       </c>
       <c r="N111">
-        <v>0.84084150627241505</v>
+        <v>0.85379924898806703</v>
       </c>
       <c r="O111">
         <v>0</v>
@@ -6390,7 +6390,7 @@
         <v>0.40216099999999999</v>
       </c>
       <c r="N112">
-        <v>0.84084150627241505</v>
+        <v>0.47222624056937201</v>
       </c>
       <c r="O112">
         <v>1</v>
@@ -6443,7 +6443,7 @@
         <v>0.273789</v>
       </c>
       <c r="N113">
-        <v>0.84084150627241505</v>
+        <v>0.384456261996449</v>
       </c>
       <c r="O113">
         <v>1</v>
@@ -6496,7 +6496,7 @@
         <v>0.70169199999999998</v>
       </c>
       <c r="N114">
-        <v>0.84084150627241505</v>
+        <v>0.67623190726041704</v>
       </c>
       <c r="O114">
         <v>-1</v>
@@ -6549,7 +6549,7 @@
         <v>0.91357699999999997</v>
       </c>
       <c r="N115">
-        <v>0.84084150627241505</v>
+        <v>0.86453467276067797</v>
       </c>
       <c r="O115">
         <v>-1</v>
@@ -6602,7 +6602,7 @@
         <v>0.916605</v>
       </c>
       <c r="N116">
-        <v>0.84084150627241505</v>
+        <v>0.60326833692204695</v>
       </c>
       <c r="O116">
         <v>-1</v>
@@ -6655,7 +6655,7 @@
         <v>0.67220999999999997</v>
       </c>
       <c r="N117">
-        <v>0.84084150627241505</v>
+        <v>0.82206626788662396</v>
       </c>
       <c r="O117">
         <v>0</v>
@@ -6708,7 +6708,7 @@
         <v>0.44859300000000002</v>
       </c>
       <c r="N118">
-        <v>0.84084150627241505</v>
+        <v>0.480528148326475</v>
       </c>
       <c r="O118">
         <v>1</v>
@@ -6761,7 +6761,7 @@
         <v>0.60929900000000004</v>
       </c>
       <c r="N119">
-        <v>0.84084150627241505</v>
+        <v>0.83852001039343105</v>
       </c>
       <c r="O119">
         <v>-1</v>
@@ -6814,7 +6814,7 @@
         <v>0.59532099999999999</v>
       </c>
       <c r="N120">
-        <v>0.84084150627241505</v>
+        <v>0.50237490140117103</v>
       </c>
       <c r="O120">
         <v>1</v>
@@ -6867,7 +6867,7 @@
         <v>0.74936599999999998</v>
       </c>
       <c r="N121">
-        <v>0.84084150627241505</v>
+        <v>0.70358186857579597</v>
       </c>
       <c r="O121">
         <v>1</v>
@@ -6920,7 +6920,7 @@
         <v>0.81809900000000002</v>
       </c>
       <c r="N122">
-        <v>0.84084150627241505</v>
+        <v>0.80305240836562597</v>
       </c>
       <c r="O122">
         <v>-1</v>
@@ -6973,7 +6973,7 @@
         <v>0.49788500000000002</v>
       </c>
       <c r="N123">
-        <v>0.84084150627241505</v>
+        <v>0.33112862771651802</v>
       </c>
       <c r="O123">
         <v>0</v>
@@ -7026,7 +7026,7 @@
         <v>0.56981400000000004</v>
       </c>
       <c r="N124">
-        <v>0.84084150627241505</v>
+        <v>0.61768806991667602</v>
       </c>
       <c r="O124">
         <v>1</v>
@@ -7079,7 +7079,7 @@
         <v>0.690689</v>
       </c>
       <c r="N125">
-        <v>0.84084150627241505</v>
+        <v>0.82935697049579504</v>
       </c>
       <c r="O125">
         <v>-1</v>
@@ -7132,7 +7132,7 @@
         <v>0.540238</v>
       </c>
       <c r="N126">
-        <v>0.84084150627241505</v>
+        <v>0.42800423324450898</v>
       </c>
       <c r="O126">
         <v>0</v>
@@ -7185,7 +7185,7 @@
         <v>0.50019800000000003</v>
       </c>
       <c r="N127">
-        <v>0.84084150627241505</v>
+        <v>0.63854902350328302</v>
       </c>
       <c r="O127">
         <v>1</v>
@@ -7238,7 +7238,7 @@
         <v>0.45644000000000001</v>
       </c>
       <c r="N128">
-        <v>0.84084150627241505</v>
+        <v>0.26063267364919501</v>
       </c>
       <c r="O128">
         <v>0</v>
@@ -7291,7 +7291,7 @@
         <v>0.60978200000000005</v>
       </c>
       <c r="N129">
-        <v>0.84084150627241505</v>
+        <v>0.52126364456721697</v>
       </c>
       <c r="O129">
         <v>1</v>
@@ -7344,7 +7344,7 @@
         <v>0.61493399999999998</v>
       </c>
       <c r="N130">
-        <v>0.84084150627241505</v>
+        <v>0.59205704811748805</v>
       </c>
       <c r="O130">
         <v>1</v>
@@ -7397,7 +7397,7 @@
         <v>0.40868399999999999</v>
       </c>
       <c r="N131">
-        <v>0.84084150627241505</v>
+        <v>0.35639735469240003</v>
       </c>
       <c r="O131">
         <v>0</v>
@@ -7450,7 +7450,7 @@
         <v>0.43621599999999999</v>
       </c>
       <c r="N132">
-        <v>0.84084150627241505</v>
+        <v>0.71195971690062398</v>
       </c>
       <c r="O132">
         <v>-1</v>
@@ -7503,7 +7503,7 @@
         <v>0.62883599999999995</v>
       </c>
       <c r="N133">
-        <v>0.84084150627241505</v>
+        <v>0.62340917484720804</v>
       </c>
       <c r="O133">
         <v>-1</v>
@@ -7556,7 +7556,7 @@
         <v>0.47683500000000001</v>
       </c>
       <c r="N134">
-        <v>0.84084150627241505</v>
+        <v>0.55852785245043901</v>
       </c>
       <c r="O134">
         <v>1</v>
@@ -7609,7 +7609,7 @@
         <v>0.468032</v>
       </c>
       <c r="N135">
-        <v>0.84084150627241505</v>
+        <v>0.52881878529549498</v>
       </c>
       <c r="O135">
         <v>0</v>
@@ -7662,7 +7662,7 @@
         <v>0.94131600000000004</v>
       </c>
       <c r="N136">
-        <v>0.84084150627241505</v>
+        <v>0.89305762048887305</v>
       </c>
       <c r="O136">
         <v>0</v>
@@ -7715,7 +7715,7 @@
         <v>0.53316799999999998</v>
       </c>
       <c r="N137">
-        <v>0.84084150627241505</v>
+        <v>0.54889341322872498</v>
       </c>
       <c r="O137">
         <v>1</v>
@@ -7768,7 +7768,7 @@
         <v>0.34003800000000001</v>
       </c>
       <c r="N138">
-        <v>0.84084150627241505</v>
+        <v>0.64367693265973702</v>
       </c>
       <c r="O138">
         <v>-1</v>
@@ -7821,7 +7821,7 @@
         <v>0.62978800000000001</v>
       </c>
       <c r="N139">
-        <v>0.84084150627241505</v>
+        <v>0.75418370371511401</v>
       </c>
       <c r="O139">
         <v>-1</v>
@@ -7874,7 +7874,7 @@
         <v>0.49876500000000001</v>
       </c>
       <c r="N140">
-        <v>0.84084150627241505</v>
+        <v>0.77841977008281704</v>
       </c>
       <c r="O140">
         <v>-1</v>
@@ -7927,7 +7927,7 @@
         <v>1.089534</v>
       </c>
       <c r="N141">
-        <v>0.84084150627241505</v>
+        <v>0.85266667666178497</v>
       </c>
       <c r="O141">
         <v>-1</v>
@@ -7980,7 +7980,7 @@
         <v>0.72100799999999998</v>
       </c>
       <c r="N142">
-        <v>0.84084150627241505</v>
+        <v>0.79871185644087805</v>
       </c>
       <c r="O142">
         <v>-1</v>
@@ -8033,7 +8033,7 @@
         <v>0.79668499999999998</v>
       </c>
       <c r="N143">
-        <v>0.84084150627241505</v>
+        <v>0.77698243929752397</v>
       </c>
       <c r="O143">
         <v>-1</v>
@@ -8086,7 +8086,7 @@
         <v>1.0603800000000001</v>
       </c>
       <c r="N144">
-        <v>0.84084150627241505</v>
+        <v>0.66254503116430397</v>
       </c>
       <c r="O144">
         <v>-1</v>
@@ -8139,7 +8139,7 @@
         <v>0.74786600000000003</v>
       </c>
       <c r="N145">
-        <v>0.84084150627241505</v>
+        <v>0.843665310979826</v>
       </c>
       <c r="O145">
         <v>-1</v>
@@ -8192,7 +8192,7 @@
         <v>0.389627</v>
       </c>
       <c r="N146">
-        <v>0.84084150627241505</v>
+        <v>0.248912506457344</v>
       </c>
       <c r="O146">
         <v>1</v>
@@ -8245,7 +8245,7 @@
         <v>0.80556300000000003</v>
       </c>
       <c r="N147">
-        <v>0.84084150627241505</v>
+        <v>0.79307196505007904</v>
       </c>
       <c r="O147">
         <v>-1</v>
@@ -8298,7 +8298,7 @@
         <v>0.63346499999999994</v>
       </c>
       <c r="N148">
-        <v>0.84084150627241505</v>
+        <v>0.64019866703518102</v>
       </c>
       <c r="O148">
         <v>1</v>
@@ -8351,7 +8351,7 @@
         <v>0.64243700000000004</v>
       </c>
       <c r="N149">
-        <v>0.84084150627241505</v>
+        <v>0.71563160000347903</v>
       </c>
       <c r="O149">
         <v>-1</v>
@@ -8404,7 +8404,7 @@
         <v>0.71341100000000002</v>
       </c>
       <c r="N150">
-        <v>0.84084150627241505</v>
+        <v>0.61423123209577501</v>
       </c>
       <c r="O150">
         <v>-1</v>
@@ -8457,7 +8457,7 @@
         <v>0.69118199999999996</v>
       </c>
       <c r="N151">
-        <v>0.84084150627241505</v>
+        <v>0.61614190558398096</v>
       </c>
       <c r="O151">
         <v>1</v>
@@ -8510,7 +8510,7 @@
         <v>0.36956299999999997</v>
       </c>
       <c r="N152">
-        <v>0.84084150627241505</v>
+        <v>0.61026051374678403</v>
       </c>
       <c r="O152">
         <v>-1</v>
@@ -8563,7 +8563,7 @@
         <v>0.56158600000000003</v>
       </c>
       <c r="N153">
-        <v>0.84084150627241505</v>
+        <v>0.81981400172089203</v>
       </c>
       <c r="O153">
         <v>-1</v>
@@ -8616,7 +8616,7 @@
         <v>0.32301000000000002</v>
       </c>
       <c r="N154">
-        <v>0.84084150627241505</v>
+        <v>0.44678900555760898</v>
       </c>
       <c r="O154">
         <v>1</v>
@@ -8669,7 +8669,7 @@
         <v>0.39857700000000001</v>
       </c>
       <c r="N155">
-        <v>0.84084150627241505</v>
+        <v>0.42820759639129402</v>
       </c>
       <c r="O155">
         <v>1</v>
@@ -8722,7 +8722,7 @@
         <v>0.688411</v>
       </c>
       <c r="N156">
-        <v>0.84084150627241505</v>
+        <v>0.79530860218091304</v>
       </c>
       <c r="O156">
         <v>-1</v>
@@ -8775,7 +8775,7 @@
         <v>0.51523399999999997</v>
       </c>
       <c r="N157">
-        <v>0.84084150627241505</v>
+        <v>0.64886596904590699</v>
       </c>
       <c r="O157">
         <v>-1</v>
@@ -8828,7 +8828,7 @@
         <v>0.818824</v>
       </c>
       <c r="N158">
-        <v>0.84084150627241505</v>
+        <v>0.68122908279016803</v>
       </c>
       <c r="O158">
         <v>-1</v>
@@ -8881,7 +8881,7 @@
         <v>0.67451700000000003</v>
       </c>
       <c r="N159">
-        <v>0.84084150627241505</v>
+        <v>0.63417869463390497</v>
       </c>
       <c r="O159">
         <v>-1</v>
@@ -8934,7 +8934,7 @@
         <v>0.63548700000000002</v>
       </c>
       <c r="N160">
-        <v>0.84084150627241505</v>
+        <v>0.61949712893750997</v>
       </c>
       <c r="O160">
         <v>-1</v>
@@ -8987,7 +8987,7 @@
         <v>0.73807500000000004</v>
       </c>
       <c r="N161">
-        <v>0.84084150627241505</v>
+        <v>0.66027651607954196</v>
       </c>
       <c r="O161">
         <v>-1</v>
@@ -9040,7 +9040,7 @@
         <v>0.76509300000000002</v>
       </c>
       <c r="N162">
-        <v>0.84084150627241505</v>
+        <v>0.61135687189324495</v>
       </c>
       <c r="O162">
         <v>-1</v>
@@ -9093,7 +9093,7 @@
         <v>0.54419899999999999</v>
       </c>
       <c r="N163">
-        <v>0.84084150627241505</v>
+        <v>0.818192734720813</v>
       </c>
       <c r="O163">
         <v>-1</v>
@@ -9146,7 +9146,7 @@
         <v>0.84890500000000002</v>
       </c>
       <c r="N164">
-        <v>0.84084150627241505</v>
+        <v>0.85197631550462105</v>
       </c>
       <c r="O164">
         <v>-1</v>
@@ -9199,7 +9199,7 @@
         <v>1.001862</v>
       </c>
       <c r="N165">
-        <v>0.84084150627241505</v>
+        <v>0.834227695486916</v>
       </c>
       <c r="O165">
         <v>-1</v>
@@ -9252,7 +9252,7 @@
         <v>1.0196700000000001</v>
       </c>
       <c r="N166">
-        <v>0.84084150627241505</v>
+        <v>0.851089852907152</v>
       </c>
       <c r="O166">
         <v>0</v>
@@ -9305,7 +9305,7 @@
         <v>0.34209099999999998</v>
       </c>
       <c r="N167">
-        <v>0.84084150627241505</v>
+        <v>0.45758524201575601</v>
       </c>
       <c r="O167">
         <v>1</v>
@@ -9358,7 +9358,7 @@
         <v>0.77047600000000005</v>
       </c>
       <c r="N168">
-        <v>0.84084150627241505</v>
+        <v>0.70261700627236801</v>
       </c>
       <c r="O168">
         <v>-1</v>
@@ -9411,7 +9411,7 @@
         <v>0.50171299999999996</v>
       </c>
       <c r="N169">
-        <v>0.84084150627241505</v>
+        <v>0.53575685660900396</v>
       </c>
       <c r="O169">
         <v>1</v>
@@ -9464,7 +9464,7 @@
         <v>0.70894699999999999</v>
       </c>
       <c r="N170">
-        <v>0.84084150627241505</v>
+        <v>0.74507638699458301</v>
       </c>
       <c r="O170">
         <v>-1</v>
@@ -9517,7 +9517,7 @@
         <v>0.63095500000000004</v>
       </c>
       <c r="N171">
-        <v>0.84084150627241505</v>
+        <v>0.66262750015244698</v>
       </c>
       <c r="O171">
         <v>-1</v>
@@ -9570,7 +9570,7 @@
         <v>0.93206599999999995</v>
       </c>
       <c r="N172">
-        <v>0.84084150627241505</v>
+        <v>0.754713486043325</v>
       </c>
       <c r="O172">
         <v>-1</v>
@@ -9623,7 +9623,7 @@
         <v>0.40276099999999998</v>
       </c>
       <c r="N173">
-        <v>0.84084150627241505</v>
+        <v>0.75448856917687401</v>
       </c>
       <c r="O173">
         <v>-1</v>
@@ -9676,7 +9676,7 @@
         <v>0.45176300000000003</v>
       </c>
       <c r="N174">
-        <v>0.84084150627241505</v>
+        <v>0.48546310937731502</v>
       </c>
       <c r="O174">
         <v>1</v>
@@ -9729,7 +9729,7 @@
         <v>1.0139180000000001</v>
       </c>
       <c r="N175">
-        <v>0.84084150627241505</v>
+        <v>0.79912250833607001</v>
       </c>
       <c r="O175">
         <v>0</v>
@@ -9782,7 +9782,7 @@
         <v>0.50144100000000003</v>
       </c>
       <c r="N176">
-        <v>0.84084150627241505</v>
+        <v>0.58203680953102099</v>
       </c>
       <c r="O176">
         <v>-1</v>
@@ -9835,7 +9835,7 @@
         <v>0.471746</v>
       </c>
       <c r="N177">
-        <v>0.84084150627241505</v>
+        <v>0.44256293233783001</v>
       </c>
       <c r="O177">
         <v>1</v>
@@ -9888,7 +9888,7 @@
         <v>0.86720200000000003</v>
       </c>
       <c r="N178">
-        <v>0.84084150627241505</v>
+        <v>0.83848417151011401</v>
       </c>
       <c r="O178">
         <v>-1</v>
@@ -9941,7 +9941,7 @@
         <v>1.0482400000000001</v>
       </c>
       <c r="N179">
-        <v>0.84084150627241505</v>
+        <v>0.75310267994633895</v>
       </c>
       <c r="O179">
         <v>0</v>
@@ -9994,7 +9994,7 @@
         <v>0.87149799999999999</v>
       </c>
       <c r="N180">
-        <v>0.84084150627241505</v>
+        <v>0.89823698061754598</v>
       </c>
       <c r="O180">
         <v>-1</v>
@@ -10047,7 +10047,7 @@
         <v>0.91186400000000001</v>
       </c>
       <c r="N181">
-        <v>0.84084150627241505</v>
+        <v>0.82237438048363498</v>
       </c>
       <c r="O181">
         <v>-1</v>
@@ -10100,7 +10100,7 @@
         <v>0.48938100000000001</v>
       </c>
       <c r="N182">
-        <v>0.84084150627241505</v>
+        <v>0.38714741351426002</v>
       </c>
       <c r="O182">
         <v>1</v>
@@ -10153,7 +10153,7 @@
         <v>0.79054899999999995</v>
       </c>
       <c r="N183">
-        <v>0.84084150627241505</v>
+        <v>0.62120869466483497</v>
       </c>
       <c r="O183">
         <v>-1</v>
@@ -10206,7 +10206,7 @@
         <v>0.51223799999999997</v>
       </c>
       <c r="N184">
-        <v>0.84084150627241505</v>
+        <v>0.71019455560919598</v>
       </c>
       <c r="O184">
         <v>-1</v>
@@ -10259,7 +10259,7 @@
         <v>0.72362499999999996</v>
       </c>
       <c r="N185">
-        <v>0.84084150627241505</v>
+        <v>0.60069421275755597</v>
       </c>
       <c r="O185">
         <v>1</v>
@@ -10312,7 +10312,7 @@
         <v>0.62356900000000004</v>
       </c>
       <c r="N186">
-        <v>0.84084150627241505</v>
+        <v>0.60196780404708095</v>
       </c>
       <c r="O186">
         <v>1</v>
@@ -10365,7 +10365,7 @@
         <v>0.95103300000000002</v>
       </c>
       <c r="N187">
-        <v>0.84084150627241505</v>
+        <v>0.920354726134468</v>
       </c>
       <c r="O187">
         <v>0</v>
@@ -10418,7 +10418,7 @@
         <v>0.12624099999999999</v>
       </c>
       <c r="N188">
-        <v>0.84084150627241505</v>
+        <v>0.52915230682572001</v>
       </c>
       <c r="O188">
         <v>-1</v>
@@ -10471,7 +10471,7 @@
         <v>0.43367899999999998</v>
       </c>
       <c r="N189">
-        <v>0.84084150627241505</v>
+        <v>0.541091787017843</v>
       </c>
       <c r="O189">
         <v>1</v>
@@ -10524,7 +10524,7 @@
         <v>0.37397599999999998</v>
       </c>
       <c r="N190">
-        <v>0.84084150627241505</v>
+        <v>0.37359545682972101</v>
       </c>
       <c r="O190">
         <v>1</v>
@@ -10577,7 +10577,7 @@
         <v>0.94827499999999998</v>
       </c>
       <c r="N191">
-        <v>0.84084150627241505</v>
+        <v>0.809197060007951</v>
       </c>
       <c r="O191">
         <v>-1</v>
@@ -10630,7 +10630,7 @@
         <v>0.133827</v>
       </c>
       <c r="N192">
-        <v>0.84084150627241505</v>
+        <v>0.44883812853073302</v>
       </c>
       <c r="O192">
         <v>-1</v>
@@ -10683,7 +10683,7 @@
         <v>0.64898299999999998</v>
       </c>
       <c r="N193">
-        <v>0.84084150627241505</v>
+        <v>0.87760524567367004</v>
       </c>
       <c r="O193">
         <v>-1</v>
@@ -10736,7 +10736,7 @@
         <v>0.51972499999999999</v>
       </c>
       <c r="N194">
-        <v>0.84084150627241505</v>
+        <v>0.87283433814289502</v>
       </c>
       <c r="O194">
         <v>-1</v>
@@ -10789,7 +10789,7 @@
         <v>0.35805199999999998</v>
       </c>
       <c r="N195">
-        <v>0.84084150627241505</v>
+        <v>0.69263017396648296</v>
       </c>
       <c r="O195">
         <v>-1</v>
@@ -10842,7 +10842,7 @@
         <v>0.58022399999999996</v>
       </c>
       <c r="N196">
-        <v>0.84084150627241505</v>
+        <v>0.54666424520304102</v>
       </c>
       <c r="O196">
         <v>-1</v>
@@ -10895,7 +10895,7 @@
         <v>0.20374100000000001</v>
       </c>
       <c r="N197">
-        <v>0.84084150627241505</v>
+        <v>0.64364115492860197</v>
       </c>
       <c r="O197">
         <v>-1</v>
@@ -10948,7 +10948,7 @@
         <v>0.38680900000000001</v>
       </c>
       <c r="N198">
-        <v>0.84084150627241505</v>
+        <v>0.81738470933070895</v>
       </c>
       <c r="O198">
         <v>-1</v>
@@ -11001,7 +11001,7 @@
         <v>0.65356700000000001</v>
       </c>
       <c r="N199">
-        <v>0.84084150627241505</v>
+        <v>0.84310743706831104</v>
       </c>
       <c r="O199">
         <v>0</v>
@@ -11054,7 +11054,7 @@
         <v>0.247779</v>
       </c>
       <c r="N200">
-        <v>0.84084150627241505</v>
+        <v>0.37130726389225899</v>
       </c>
       <c r="O200">
         <v>1</v>
@@ -11107,7 +11107,7 @@
         <v>0.442411</v>
       </c>
       <c r="N201">
-        <v>0.84084150627241505</v>
+        <v>0.81964749692791405</v>
       </c>
       <c r="O201">
         <v>-1</v>
@@ -11160,7 +11160,7 @@
         <v>0.29540499999999997</v>
       </c>
       <c r="N202">
-        <v>0.84084150627241505</v>
+        <v>0.71409865609713796</v>
       </c>
       <c r="O202">
         <v>-1</v>
@@ -11213,7 +11213,7 @@
         <v>0.32301000000000002</v>
       </c>
       <c r="N203">
-        <v>0.84084150627241505</v>
+        <v>0.46562705535306198</v>
       </c>
       <c r="O203">
         <v>1</v>
@@ -11266,7 +11266,7 @@
         <v>0.41343600000000003</v>
       </c>
       <c r="N204">
-        <v>0.84084150627241505</v>
+        <v>0.317611462427623</v>
       </c>
       <c r="O204">
         <v>1</v>
@@ -11319,7 +11319,7 @@
         <v>0.35053400000000001</v>
       </c>
       <c r="N205">
-        <v>0.84084150627241505</v>
+        <v>0.46681795994090702</v>
       </c>
       <c r="O205">
         <v>1</v>
@@ -11372,7 +11372,7 @@
         <v>0.53824799999999995</v>
       </c>
       <c r="N206">
-        <v>0.84084150627241505</v>
+        <v>0.345008790459572</v>
       </c>
       <c r="O206">
         <v>0</v>
@@ -11425,7 +11425,7 @@
         <v>0.22837399999999999</v>
       </c>
       <c r="N207">
-        <v>0.84084150627241505</v>
+        <v>0.39943632214015901</v>
       </c>
       <c r="O207">
         <v>1</v>
@@ -11478,7 +11478,7 @@
         <v>0.73151500000000003</v>
       </c>
       <c r="N208">
-        <v>0.84084150627241505</v>
+        <v>0.76224579051087704</v>
       </c>
       <c r="O208">
         <v>0</v>
@@ -11531,7 +11531,7 @@
         <v>0.399617</v>
       </c>
       <c r="N209">
-        <v>0.84084150627241505</v>
+        <v>0.56366508798745396</v>
       </c>
       <c r="O209">
         <v>1</v>
@@ -11584,7 +11584,7 @@
         <v>0.77925500000000003</v>
       </c>
       <c r="N210">
-        <v>0.84084150627241505</v>
+        <v>0.91489190067721904</v>
       </c>
       <c r="O210">
         <v>0</v>
@@ -11637,7 +11637,7 @@
         <v>0.74322500000000002</v>
       </c>
       <c r="N211">
-        <v>0.84084150627241505</v>
+        <v>0.724903010627583</v>
       </c>
       <c r="O211">
         <v>0</v>
@@ -11690,7 +11690,7 @@
         <v>0.303699</v>
       </c>
       <c r="N212">
-        <v>0.84084150627241505</v>
+        <v>0.469939873387412</v>
       </c>
       <c r="O212">
         <v>1</v>
@@ -11743,7 +11743,7 @@
         <v>0.64721099999999998</v>
       </c>
       <c r="N213">
-        <v>0.84084150627241505</v>
+        <v>0.76147068874103396</v>
       </c>
       <c r="O213">
         <v>-1</v>
@@ -11796,7 +11796,7 @@
         <v>0.46736800000000001</v>
       </c>
       <c r="N214">
-        <v>0.84084150627241505</v>
+        <v>0.65765019559613702</v>
       </c>
       <c r="O214">
         <v>-1</v>
@@ -11849,7 +11849,7 @@
         <v>0.81067699999999998</v>
       </c>
       <c r="N215">
-        <v>0.84084150627241505</v>
+        <v>0.91001719798691605</v>
       </c>
       <c r="O215">
         <v>-1</v>
@@ -11902,7 +11902,7 @@
         <v>0.58474199999999998</v>
       </c>
       <c r="N216">
-        <v>0.84084150627241505</v>
+        <v>0.54422738363940903</v>
       </c>
       <c r="O216">
         <v>1</v>
@@ -11955,7 +11955,7 @@
         <v>0.25373800000000002</v>
       </c>
       <c r="N217">
-        <v>0.84084150627241505</v>
+        <v>0.53023463619286104</v>
       </c>
       <c r="O217">
         <v>1</v>
@@ -12008,7 +12008,7 @@
         <v>0.39727600000000002</v>
       </c>
       <c r="N218">
-        <v>0.84084150627241505</v>
+        <v>0.53580683868238499</v>
       </c>
       <c r="O218">
         <v>1</v>
@@ -12061,7 +12061,7 @@
         <v>1.0017750000000001</v>
       </c>
       <c r="N219">
-        <v>0.84084150627241505</v>
+        <v>0.86647578927868996</v>
       </c>
       <c r="O219">
         <v>-1</v>
@@ -12114,7 +12114,7 @@
         <v>0.74547300000000005</v>
       </c>
       <c r="N220">
-        <v>0.84084150627241505</v>
+        <v>0.75738425373324003</v>
       </c>
       <c r="O220">
         <v>-1</v>
@@ -12167,7 +12167,7 @@
         <v>0.55675399999999997</v>
       </c>
       <c r="N221">
-        <v>0.84084150627241505</v>
+        <v>0.79774385179207896</v>
       </c>
       <c r="O221">
         <v>-1</v>
@@ -12220,7 +12220,7 @@
         <v>0.68236600000000003</v>
       </c>
       <c r="N222">
-        <v>0.84084150627241505</v>
+        <v>0.72357442397902705</v>
       </c>
       <c r="O222">
         <v>-1</v>
@@ -12273,7 +12273,7 @@
         <v>0.49509799999999998</v>
       </c>
       <c r="N223">
-        <v>0.84084150627241505</v>
+        <v>0.56017122292150801</v>
       </c>
       <c r="O223">
         <v>1</v>
@@ -12326,7 +12326,7 @@
         <v>0.79521200000000003</v>
       </c>
       <c r="N224">
-        <v>0.84084150627241505</v>
+        <v>0.75580702331580796</v>
       </c>
       <c r="O224">
         <v>-1</v>
@@ -12379,7 +12379,7 @@
         <v>0.99681299999999995</v>
       </c>
       <c r="N225">
-        <v>0.84084150627241505</v>
+        <v>0.815909906400903</v>
       </c>
       <c r="O225">
         <v>0</v>
@@ -12432,7 +12432,7 @@
         <v>0.84259300000000004</v>
       </c>
       <c r="N226">
-        <v>0.84084150627241505</v>
+        <v>0.73340450036780402</v>
       </c>
       <c r="O226">
         <v>-1</v>
@@ -12485,7 +12485,7 @@
         <v>0.447019</v>
       </c>
       <c r="N227">
-        <v>0.84084150627241505</v>
+        <v>0.80888398195529998</v>
       </c>
       <c r="O227">
         <v>-1</v>
@@ -12538,7 +12538,7 @@
         <v>0.50901300000000005</v>
       </c>
       <c r="N228">
-        <v>0.84084150627241505</v>
+        <v>0.40888780473894698</v>
       </c>
       <c r="O228">
         <v>1</v>
@@ -12591,7 +12591,7 @@
         <v>0.84545800000000004</v>
       </c>
       <c r="N229">
-        <v>0.84084150627241505</v>
+        <v>0.59771193337270301</v>
       </c>
       <c r="O229">
         <v>-1</v>
@@ -12644,7 +12644,7 @@
         <v>0.42960700000000002</v>
       </c>
       <c r="N230">
-        <v>0.84084150627241505</v>
+        <v>0.414847159912965</v>
       </c>
       <c r="O230">
         <v>1</v>
@@ -12697,7 +12697,7 @@
         <v>0.92329700000000003</v>
       </c>
       <c r="N231">
-        <v>0.84084150627241505</v>
+        <v>0.76216571520699705</v>
       </c>
       <c r="O231">
         <v>-1</v>
@@ -12750,7 +12750,7 @@
         <v>0.54285899999999998</v>
       </c>
       <c r="N232">
-        <v>0.84084150627241505</v>
+        <v>0.58449749142816698</v>
       </c>
       <c r="O232">
         <v>0</v>
@@ -12803,7 +12803,7 @@
         <v>0.86543599999999998</v>
       </c>
       <c r="N233">
-        <v>0.84084150627241505</v>
+        <v>0.64746302835324598</v>
       </c>
       <c r="O233">
         <v>0</v>
@@ -12856,7 +12856,7 @@
         <v>0.48361500000000002</v>
       </c>
       <c r="N234">
-        <v>0.84084150627241505</v>
+        <v>0.72246598658493999</v>
       </c>
       <c r="O234">
         <v>-1</v>
@@ -12909,7 +12909,7 @@
         <v>0.29098099999999999</v>
       </c>
       <c r="N235">
-        <v>0.84084150627241505</v>
+        <v>0.18985041786403201</v>
       </c>
       <c r="O235">
         <v>1</v>
@@ -12962,7 +12962,7 @@
         <v>0.30926799999999999</v>
       </c>
       <c r="N236">
-        <v>0.84084150627241505</v>
+        <v>0.43145692436987398</v>
       </c>
       <c r="O236">
         <v>1</v>
@@ -13015,7 +13015,7 @@
         <v>0.46939700000000001</v>
       </c>
       <c r="N237">
-        <v>0.84084150627241505</v>
+        <v>0.59671386727886699</v>
       </c>
       <c r="O237">
         <v>1</v>
@@ -13068,7 +13068,7 @@
         <v>0.65254900000000005</v>
       </c>
       <c r="N238">
-        <v>0.84084150627241505</v>
+        <v>0.65994271993573095</v>
       </c>
       <c r="O238">
         <v>-1</v>
@@ -13121,7 +13121,7 @@
         <v>0.36947099999999999</v>
       </c>
       <c r="N239">
-        <v>0.84084150627241505</v>
+        <v>0.38375481124626898</v>
       </c>
       <c r="O239">
         <v>1</v>
@@ -13174,7 +13174,7 @@
         <v>0.93621699999999997</v>
       </c>
       <c r="N240">
-        <v>0.84084150627241505</v>
+        <v>0.90560001333439699</v>
       </c>
       <c r="O240">
         <v>-1</v>
@@ -13227,7 +13227,7 @@
         <v>0.61875999999999998</v>
       </c>
       <c r="N241">
-        <v>0.84084150627241505</v>
+        <v>0.76846540972757005</v>
       </c>
       <c r="O241">
         <v>-1</v>
@@ -13280,7 +13280,7 @@
         <v>0.88321400000000005</v>
       </c>
       <c r="N242">
-        <v>0.84084150627241505</v>
+        <v>0.83064895072753098</v>
       </c>
       <c r="O242">
         <v>0</v>
@@ -13333,7 +13333,7 @@
         <v>0.57382699999999998</v>
       </c>
       <c r="N243">
-        <v>0.84084150627241505</v>
+        <v>0.72605947203924004</v>
       </c>
       <c r="O243">
         <v>-1</v>
@@ -13386,7 +13386,7 @@
         <v>0.36483399999999999</v>
       </c>
       <c r="N244">
-        <v>0.84084150627241505</v>
+        <v>0.59589622327060499</v>
       </c>
       <c r="O244">
         <v>1</v>
@@ -13439,7 +13439,7 @@
         <v>0.559249</v>
       </c>
       <c r="N245">
-        <v>0.84084150627241505</v>
+        <v>0.79752506803230905</v>
       </c>
       <c r="O245">
         <v>-1</v>
@@ -13492,7 +13492,7 @@
         <v>0.42155399999999998</v>
       </c>
       <c r="N246">
-        <v>0.84084150627241505</v>
+        <v>0.61856662459755596</v>
       </c>
       <c r="O246">
         <v>1</v>
@@ -13545,7 +13545,7 @@
         <v>0.36409000000000002</v>
       </c>
       <c r="N247">
-        <v>0.84084150627241505</v>
+        <v>0.39322691237607899</v>
       </c>
       <c r="O247">
         <v>1</v>
@@ -13598,7 +13598,7 @@
         <v>0.63436599999999999</v>
       </c>
       <c r="N248">
-        <v>0.84084150627241505</v>
+        <v>0.74875533728778099</v>
       </c>
       <c r="O248">
         <v>-1</v>
@@ -13651,7 +13651,7 @@
         <v>0.48014699999999999</v>
       </c>
       <c r="N249">
-        <v>0.84084150627241505</v>
+        <v>0.61574598841908501</v>
       </c>
       <c r="O249">
         <v>-1</v>
@@ -13704,7 +13704,7 @@
         <v>0.67359999999999998</v>
       </c>
       <c r="N250">
-        <v>0.84084150627241505</v>
+        <v>0.82433462279803305</v>
       </c>
       <c r="O250">
         <v>-1</v>
@@ -13757,7 +13757,7 @@
         <v>0.82953699999999997</v>
       </c>
       <c r="N251">
-        <v>0.84084150627241505</v>
+        <v>0.86113166597155499</v>
       </c>
       <c r="O251">
         <v>-1</v>
@@ -13810,7 +13810,7 @@
         <v>0.370861</v>
       </c>
       <c r="N252">
-        <v>0.84084150627241505</v>
+        <v>0.34676877554484298</v>
       </c>
       <c r="O252">
         <v>1</v>
@@ -13863,7 +13863,7 @@
         <v>0.46070100000000003</v>
       </c>
       <c r="N253">
-        <v>0.84084150627241505</v>
+        <v>0.80579324763984705</v>
       </c>
       <c r="O253">
         <v>-1</v>
@@ -13916,7 +13916,7 @@
         <v>0.78869199999999995</v>
       </c>
       <c r="N254">
-        <v>0.84084150627241505</v>
+        <v>0.89346874634982099</v>
       </c>
       <c r="O254">
         <v>-1</v>
@@ -13969,7 +13969,7 @@
         <v>0.26905400000000002</v>
       </c>
       <c r="N255">
-        <v>0.84084150627241505</v>
+        <v>0.52835051779769304</v>
       </c>
       <c r="O255">
         <v>1</v>
@@ -14022,7 +14022,7 @@
         <v>0.40211000000000002</v>
       </c>
       <c r="N256">
-        <v>0.84084150627241505</v>
+        <v>0.31612221643963501</v>
       </c>
       <c r="O256">
         <v>1</v>
@@ -14075,7 +14075,7 @@
         <v>0.54885300000000004</v>
       </c>
       <c r="N257">
-        <v>0.84084150627241505</v>
+        <v>0.78829035451771601</v>
       </c>
       <c r="O257">
         <v>-1</v>
@@ -14128,7 +14128,7 @@
         <v>0.23298199999999999</v>
       </c>
       <c r="N258">
-        <v>0.84084150627241505</v>
+        <v>0.96537886105192605</v>
       </c>
       <c r="O258">
         <v>-1</v>
@@ -14181,7 +14181,7 @@
         <v>0.411468</v>
       </c>
       <c r="N259">
-        <v>0.84084150627241505</v>
+        <v>0.78039800373058799</v>
       </c>
       <c r="O259">
         <v>-1</v>
@@ -14234,7 +14234,7 @@
         <v>0.35033900000000001</v>
       </c>
       <c r="N260">
-        <v>0.84084150627241505</v>
+        <v>0.95107198061679699</v>
       </c>
       <c r="O260">
         <v>-1</v>
@@ -14287,7 +14287,7 @@
         <v>0.51072200000000001</v>
       </c>
       <c r="N261">
-        <v>0.84084150627241505</v>
+        <v>0.12250574473351</v>
       </c>
       <c r="O261">
         <v>0</v>
@@ -14340,7 +14340,7 @@
         <v>0.126219</v>
       </c>
       <c r="N262">
-        <v>0.84084150627241505</v>
+        <v>0.208494987382119</v>
       </c>
       <c r="O262">
         <v>0</v>
@@ -14393,7 +14393,7 @@
         <v>0.251448</v>
       </c>
       <c r="N263">
-        <v>0.84084150627241505</v>
+        <v>0.65160080528832798</v>
       </c>
       <c r="O263">
         <v>1</v>
@@ -14446,7 +14446,7 @@
         <v>0.28951300000000002</v>
       </c>
       <c r="N264">
-        <v>0.84084150627241505</v>
+        <v>0.85550339556392196</v>
       </c>
       <c r="O264">
         <v>0</v>
@@ -14499,7 +14499,7 @@
         <v>0.35526600000000003</v>
       </c>
       <c r="N265">
-        <v>0.84084150627241505</v>
+        <v>0.69339621716844602</v>
       </c>
       <c r="O265">
         <v>-1</v>
@@ -14552,7 +14552,7 @@
         <v>0.30299399999999999</v>
       </c>
       <c r="N266">
-        <v>0.84084150627241505</v>
+        <v>0.44043597733883499</v>
       </c>
       <c r="O266">
         <v>1</v>
@@ -14605,7 +14605,7 @@
         <v>0.29311999999999999</v>
       </c>
       <c r="N267">
-        <v>0.84084150627241505</v>
+        <v>0.34307183146745601</v>
       </c>
       <c r="O267">
         <v>1</v>
@@ -14658,7 +14658,7 @@
         <v>0.33713599999999999</v>
       </c>
       <c r="N268">
-        <v>0.84084150627241505</v>
+        <v>0.67196111146420601</v>
       </c>
       <c r="O268">
         <v>-1</v>
@@ -14711,7 +14711,7 @@
         <v>0.31711600000000001</v>
       </c>
       <c r="N269">
-        <v>0.84084150627241505</v>
+        <v>0.67633000132847398</v>
       </c>
       <c r="O269">
         <v>-1</v>
@@ -14764,7 +14764,7 @@
         <v>0.31565900000000002</v>
       </c>
       <c r="N270">
-        <v>0.84084150627241505</v>
+        <v>0.68359854906813899</v>
       </c>
       <c r="O270">
         <v>-1</v>
@@ -14817,7 +14817,7 @@
         <v>0.39764300000000002</v>
       </c>
       <c r="N271">
-        <v>0.84084150627241505</v>
+        <v>0.71173483051692998</v>
       </c>
       <c r="O271">
         <v>-1</v>
@@ -14870,7 +14870,7 @@
         <v>0.30647799999999997</v>
       </c>
       <c r="N272">
-        <v>0.84084150627241505</v>
+        <v>0.465669591067358</v>
       </c>
       <c r="O272">
         <v>1</v>
@@ -14923,7 +14923,7 @@
         <v>0.13883100000000001</v>
       </c>
       <c r="N273">
-        <v>0.84084150627241505</v>
+        <v>0.36818653728413298</v>
       </c>
       <c r="O273">
         <v>0</v>
@@ -14976,7 +14976,7 @@
         <v>0.32277400000000001</v>
       </c>
       <c r="N274">
-        <v>0.84084150627241505</v>
+        <v>0.46721534632376499</v>
       </c>
       <c r="O274">
         <v>1</v>
@@ -15029,7 +15029,7 @@
         <v>0.30529200000000001</v>
       </c>
       <c r="N275">
-        <v>0.84084150627241505</v>
+        <v>0.51662814789148503</v>
       </c>
       <c r="O275">
         <v>1</v>
@@ -15082,7 +15082,7 @@
         <v>0.32488800000000001</v>
       </c>
       <c r="N276">
-        <v>0.84084150627241505</v>
+        <v>0.45002968901135498</v>
       </c>
       <c r="O276">
         <v>1</v>
@@ -15135,7 +15135,7 @@
         <v>0.16306899999999999</v>
       </c>
       <c r="N277">
-        <v>0.84084150627241505</v>
+        <v>0.36819298058913102</v>
       </c>
       <c r="O277">
         <v>1</v>
@@ -15188,7 +15188,7 @@
         <v>0.36260300000000001</v>
       </c>
       <c r="N278">
-        <v>0.84084150627241505</v>
+        <v>0.69708101620511098</v>
       </c>
       <c r="O278">
         <v>1</v>
@@ -15241,7 +15241,7 @@
         <v>0.36057400000000001</v>
       </c>
       <c r="N279">
-        <v>0.84084150627241505</v>
+        <v>0.74562206633592598</v>
       </c>
       <c r="O279">
         <v>-1</v>
@@ -15294,7 +15294,7 @@
         <v>0.25780199999999998</v>
       </c>
       <c r="N280">
-        <v>0.84084150627241505</v>
+        <v>0.69449486217074696</v>
       </c>
       <c r="O280">
         <v>-1</v>
@@ -15347,7 +15347,7 @@
         <v>0.29264800000000002</v>
       </c>
       <c r="N281">
-        <v>0.84084150627241505</v>
+        <v>0.39226259565841798</v>
       </c>
       <c r="O281">
         <v>1</v>
@@ -15400,7 +15400,7 @@
         <v>0.226358</v>
       </c>
       <c r="N282">
-        <v>0.84084150627241505</v>
+        <v>0.49133096991692499</v>
       </c>
       <c r="O282">
         <v>1</v>
@@ -15453,7 +15453,7 @@
         <v>0.233817</v>
       </c>
       <c r="N283">
-        <v>0.84084150627241505</v>
+        <v>0.28048813495595898</v>
       </c>
       <c r="O283">
         <v>1</v>
@@ -15506,7 +15506,7 @@
         <v>0.27709899999999998</v>
       </c>
       <c r="N284">
-        <v>0.84084150627241505</v>
+        <v>0.73015633996185403</v>
       </c>
       <c r="O284">
         <v>-1</v>
@@ -15559,7 +15559,7 @@
         <v>0.23163300000000001</v>
       </c>
       <c r="N285">
-        <v>0.84084150627241505</v>
+        <v>0.39975615933637398</v>
       </c>
       <c r="O285">
         <v>1</v>
@@ -15612,7 +15612,7 @@
         <v>0.21481900000000001</v>
       </c>
       <c r="N286">
-        <v>0.84084150627241505</v>
+        <v>0.64611262550952298</v>
       </c>
       <c r="O286">
         <v>1</v>
@@ -15665,7 +15665,7 @@
         <v>0.289933</v>
       </c>
       <c r="N287">
-        <v>0.84084150627241505</v>
+        <v>0.35195060697678299</v>
       </c>
       <c r="O287">
         <v>1</v>
@@ -15718,7 +15718,7 @@
         <v>0.215447</v>
       </c>
       <c r="N288">
-        <v>0.84084150627241505</v>
+        <v>0.41573769124445997</v>
       </c>
       <c r="O288">
         <v>1</v>
@@ -15771,7 +15771,7 @@
         <v>0.19738900000000001</v>
       </c>
       <c r="N289">
-        <v>0.84084150627241505</v>
+        <v>0.25160321759766202</v>
       </c>
       <c r="O289">
         <v>1</v>
@@ -15824,7 +15824,7 @@
         <v>0.11890100000000001</v>
       </c>
       <c r="N290">
-        <v>0.84084150627241505</v>
+        <v>0.20839054055070499</v>
       </c>
       <c r="O290">
         <v>1</v>
@@ -15877,7 +15877,7 @@
         <v>0.36174899999999999</v>
       </c>
       <c r="N291">
-        <v>0.84084150627241505</v>
+        <v>0.81044746389318401</v>
       </c>
       <c r="O291">
         <v>-1</v>
@@ -15930,7 +15930,7 @@
         <v>0.40384700000000001</v>
       </c>
       <c r="N292">
-        <v>0.84084150627241505</v>
+        <v>0.58785683483763496</v>
       </c>
       <c r="O292">
         <v>0</v>
@@ -15983,7 +15983,7 @@
         <v>0.107403</v>
       </c>
       <c r="N293">
-        <v>0.84084150627241505</v>
+        <v>0.29135754718265799</v>
       </c>
       <c r="O293">
         <v>1</v>
@@ -16036,7 +16036,7 @@
         <v>0.37130999999999997</v>
       </c>
       <c r="N294">
-        <v>0.84084150627241505</v>
+        <v>0.50150210442174303</v>
       </c>
       <c r="O294">
         <v>1</v>
@@ -16089,7 +16089,7 @@
         <v>0.22920299999999999</v>
       </c>
       <c r="N295">
-        <v>0.84084150627241505</v>
+        <v>0.485441956843147</v>
       </c>
       <c r="O295">
         <v>0</v>
@@ -16142,7 +16142,7 @@
         <v>0.21693399999999999</v>
       </c>
       <c r="N296">
-        <v>0.84084150627241505</v>
+        <v>0.38445287219832402</v>
       </c>
       <c r="O296">
         <v>1</v>
@@ -16195,7 +16195,7 @@
         <v>0.225659</v>
       </c>
       <c r="N297">
-        <v>0.84084150627241505</v>
+        <v>0.35171599277214899</v>
       </c>
       <c r="O297">
         <v>1</v>
@@ -16248,7 +16248,7 @@
         <v>0.37786199999999998</v>
       </c>
       <c r="N298">
-        <v>0.84084150627241505</v>
+        <v>0.80013665267524403</v>
       </c>
       <c r="O298">
         <v>0</v>
@@ -16301,7 +16301,7 @@
         <v>0.14954899999999999</v>
       </c>
       <c r="N299">
-        <v>0.84084150627241505</v>
+        <v>0.53877380131261199</v>
       </c>
       <c r="O299">
         <v>1</v>
@@ -16354,7 +16354,7 @@
         <v>0.17280300000000001</v>
       </c>
       <c r="N300">
-        <v>0.84084150627241505</v>
+        <v>0.47848744672141602</v>
       </c>
       <c r="O300">
         <v>1</v>
@@ -16407,7 +16407,7 @@
         <v>0.12940099999999999</v>
       </c>
       <c r="N301">
-        <v>0.84084150627241505</v>
+        <v>0.31568705610999398</v>
       </c>
       <c r="O301">
         <v>0</v>
@@ -16460,7 +16460,7 @@
         <v>0.39044000000000001</v>
       </c>
       <c r="N302">
-        <v>0.84084150627241505</v>
+        <v>0.53270280491643895</v>
       </c>
       <c r="O302">
         <v>1</v>
@@ -16513,7 +16513,7 @@
         <v>0.38000200000000001</v>
       </c>
       <c r="N303">
-        <v>0.84084150627241505</v>
+        <v>0.95045533195819898</v>
       </c>
       <c r="O303">
         <v>-1</v>
@@ -16566,7 +16566,7 @@
         <v>0.234268</v>
       </c>
       <c r="N304">
-        <v>0.84084150627241505</v>
+        <v>0.84624151328151997</v>
       </c>
       <c r="O304">
         <v>-1</v>
@@ -16619,7 +16619,7 @@
         <v>0.31108000000000002</v>
       </c>
       <c r="N305">
-        <v>0.84084150627241505</v>
+        <v>0.39041972793666502</v>
       </c>
       <c r="O305">
         <v>1</v>
@@ -16672,7 +16672,7 @@
         <v>0.440249</v>
       </c>
       <c r="N306">
-        <v>0.84084150627241505</v>
+        <v>0.40699404922883597</v>
       </c>
       <c r="O306">
         <v>0</v>
@@ -16725,7 +16725,7 @@
         <v>0.41120000000000001</v>
       </c>
       <c r="N307">
-        <v>0.84084150627241505</v>
+        <v>0.34444626826414798</v>
       </c>
       <c r="O307">
         <v>0</v>
@@ -16778,7 +16778,7 @@
         <v>0.212862</v>
       </c>
       <c r="N308">
-        <v>0.84084150627241505</v>
+        <v>0.59687061277864895</v>
       </c>
       <c r="O308">
         <v>0</v>
@@ -16831,7 +16831,7 @@
         <v>0.14175499999999999</v>
       </c>
       <c r="N309">
-        <v>0.84084150627241505</v>
+        <v>0.56181363697980402</v>
       </c>
       <c r="O309">
         <v>1</v>
@@ -16884,7 +16884,7 @@
         <v>0.34518599999999999</v>
       </c>
       <c r="N310">
-        <v>0.84084150627241505</v>
+        <v>0.75335384278588302</v>
       </c>
       <c r="O310">
         <v>0</v>
@@ -16937,7 +16937,7 @@
         <v>0.218003</v>
       </c>
       <c r="N311">
-        <v>0.84084150627241505</v>
+        <v>0.57284100505570601</v>
       </c>
       <c r="O311">
         <v>1</v>
@@ -16990,7 +16990,7 @@
         <v>0.20136499999999999</v>
       </c>
       <c r="N312">
-        <v>0.84084150627241505</v>
+        <v>0.38361453607971202</v>
       </c>
       <c r="O312">
         <v>0</v>
@@ -17043,7 +17043,7 @@
         <v>0.53998000000000002</v>
       </c>
       <c r="N313">
-        <v>0.84084150627241505</v>
+        <v>0.92466298414453296</v>
       </c>
       <c r="O313">
         <v>0</v>
@@ -17096,7 +17096,7 @@
         <v>0.19045699999999999</v>
       </c>
       <c r="N314">
-        <v>0.84084150627241505</v>
+        <v>0.55463495984565103</v>
       </c>
       <c r="O314">
         <v>0</v>
@@ -17149,7 +17149,7 @@
         <v>0.35363299999999998</v>
       </c>
       <c r="N315">
-        <v>0.84084150627241505</v>
+        <v>0.74400099598801195</v>
       </c>
       <c r="O315">
         <v>0</v>
@@ -17202,7 +17202,7 @@
         <v>0.19952900000000001</v>
       </c>
       <c r="N316">
-        <v>0.84084150627241505</v>
+        <v>0.62062119101463198</v>
       </c>
       <c r="O316">
         <v>1</v>
@@ -17255,7 +17255,7 @@
         <v>0.16577800000000001</v>
       </c>
       <c r="N317">
-        <v>0.84084150627241505</v>
+        <v>0.60757829213125403</v>
       </c>
       <c r="O317">
         <v>1</v>
@@ -17308,7 +17308,7 @@
         <v>0.14324200000000001</v>
       </c>
       <c r="N318">
-        <v>0.84084150627241505</v>
+        <v>0.34216312367549701</v>
       </c>
       <c r="O318">
         <v>0</v>
@@ -17361,7 +17361,7 @@
         <v>0.89853300000000003</v>
       </c>
       <c r="N319">
-        <v>0.84084150627241505</v>
+        <v>0.683775923352827</v>
       </c>
       <c r="O319">
         <v>0</v>
@@ -17414,7 +17414,7 @@
         <v>0.21518000000000001</v>
       </c>
       <c r="N320">
-        <v>0.84084150627241505</v>
+        <v>0.732015766698075</v>
       </c>
       <c r="O320">
         <v>0</v>
@@ -17467,7 +17467,7 @@
         <v>0.52196900000000002</v>
       </c>
       <c r="N321">
-        <v>0.84084150627241505</v>
+        <v>0.44971963058098602</v>
       </c>
       <c r="O321">
         <v>1</v>
@@ -17520,7 +17520,7 @@
         <v>0.69974899999999995</v>
       </c>
       <c r="N322">
-        <v>0.84084150627241505</v>
+        <v>0.65312417660446398</v>
       </c>
       <c r="O322">
         <v>1</v>
@@ -17573,7 +17573,7 @@
         <v>0.58631299999999997</v>
       </c>
       <c r="N323">
-        <v>0.84084150627241505</v>
+        <v>0.496902073201067</v>
       </c>
       <c r="O323">
         <v>1</v>
@@ -17626,7 +17626,7 @@
         <v>0.56823299999999999</v>
       </c>
       <c r="N324">
-        <v>0.84084150627241505</v>
+        <v>0.49740709285058099</v>
       </c>
       <c r="O324">
         <v>1</v>
@@ -17679,7 +17679,7 @@
         <v>0.51575700000000002</v>
       </c>
       <c r="N325">
-        <v>0.84084150627241505</v>
+        <v>0.47034119973583299</v>
       </c>
       <c r="O325">
         <v>1</v>
@@ -17732,7 +17732,7 @@
         <v>0.63286500000000001</v>
       </c>
       <c r="N326">
-        <v>0.84084150627241505</v>
+        <v>0.67541918316884797</v>
       </c>
       <c r="O326">
         <v>-1</v>
@@ -17785,7 +17785,7 @@
         <v>0.590117</v>
       </c>
       <c r="N327">
-        <v>0.84084150627241505</v>
+        <v>0.493113313395729</v>
       </c>
       <c r="O327">
         <v>1</v>
@@ -17838,7 +17838,7 @@
         <v>0.60532399999999997</v>
       </c>
       <c r="N328">
-        <v>0.84084150627241505</v>
+        <v>0.604370249685521</v>
       </c>
       <c r="O328">
         <v>-1</v>
@@ -17891,7 +17891,7 @@
         <v>0.51477499999999998</v>
       </c>
       <c r="N329">
-        <v>0.84084150627241505</v>
+        <v>0.48151318275523097</v>
       </c>
       <c r="O329">
         <v>1</v>
@@ -17944,7 +17944,7 @@
         <v>0.87026199999999998</v>
       </c>
       <c r="N330">
-        <v>0.84084150627241505</v>
+        <v>0.64935350341189801</v>
       </c>
       <c r="O330">
         <v>-1</v>
@@ -17997,7 +17997,7 @@
         <v>0.21717800000000001</v>
       </c>
       <c r="N331">
-        <v>0.84084150627241505</v>
+        <v>0.28981804899112601</v>
       </c>
       <c r="O331">
         <v>1</v>
@@ -18050,7 +18050,7 @@
         <v>0.61905100000000002</v>
       </c>
       <c r="N332">
-        <v>0.84084150627241505</v>
+        <v>0.610340756799156</v>
       </c>
       <c r="O332">
         <v>1</v>
@@ -18103,7 +18103,7 @@
         <v>0.62118600000000002</v>
       </c>
       <c r="N333">
-        <v>0.84084150627241505</v>
+        <v>0.62729494330995805</v>
       </c>
       <c r="O333">
         <v>-1</v>
@@ -18156,7 +18156,7 @@
         <v>0.66219099999999997</v>
       </c>
       <c r="N334">
-        <v>0.84084150627241505</v>
+        <v>0.62256709549572398</v>
       </c>
       <c r="O334">
         <v>1</v>
@@ -18209,7 +18209,7 @@
         <v>0.61749600000000004</v>
       </c>
       <c r="N335">
-        <v>0.84084150627241505</v>
+        <v>0.50661369036475101</v>
       </c>
       <c r="O335">
         <v>1</v>
@@ -18262,7 +18262,7 @@
         <v>0.55945199999999995</v>
       </c>
       <c r="N336">
-        <v>0.84084150627241505</v>
+        <v>0.579135334953643</v>
       </c>
       <c r="O336">
         <v>-1</v>
@@ -18315,7 +18315,7 @@
         <v>0.31831599999999999</v>
       </c>
       <c r="N337">
-        <v>0.84084150627241505</v>
+        <v>0.95243403399777304</v>
       </c>
       <c r="O337">
         <v>-1</v>
@@ -18368,7 +18368,7 @@
         <v>0.380463</v>
       </c>
       <c r="N338">
-        <v>0.84084150627241505</v>
+        <v>0.77210743471166199</v>
       </c>
       <c r="O338">
         <v>-1</v>
@@ -18421,7 +18421,7 @@
         <v>0.41991800000000001</v>
       </c>
       <c r="N339">
-        <v>0.84084150627241505</v>
+        <v>0.59916681827868401</v>
       </c>
       <c r="O339">
         <v>-1</v>
@@ -18474,7 +18474,7 @@
         <v>0.32137300000000002</v>
       </c>
       <c r="N340">
-        <v>0.84084150627241505</v>
+        <v>0.38896664987193902</v>
       </c>
       <c r="O340">
         <v>1</v>
@@ -18527,7 +18527,7 @@
         <v>0.331984</v>
       </c>
       <c r="N341">
-        <v>0.84084150627241505</v>
+        <v>0.43076861587691001</v>
       </c>
       <c r="O341">
         <v>1</v>
@@ -18580,7 +18580,7 @@
         <v>0.78470700000000004</v>
       </c>
       <c r="N342">
-        <v>0.84084150627241505</v>
+        <v>0.74212660922391804</v>
       </c>
       <c r="O342">
         <v>0</v>
@@ -18633,7 +18633,7 @@
         <v>0.50149600000000005</v>
       </c>
       <c r="N343">
-        <v>0.84084150627241505</v>
+        <v>0.60430901496123002</v>
       </c>
       <c r="O343">
         <v>0</v>
@@ -18686,7 +18686,7 @@
         <v>0.71543800000000002</v>
       </c>
       <c r="N344">
-        <v>0.84084150627241505</v>
+        <v>0.73190636021294497</v>
       </c>
       <c r="O344">
         <v>0</v>
@@ -18739,7 +18739,7 @@
         <v>0.18908800000000001</v>
       </c>
       <c r="N345">
-        <v>0.84084150627241505</v>
+        <v>0.29393976994106202</v>
       </c>
       <c r="O345">
         <v>1</v>
@@ -18792,7 +18792,7 @@
         <v>0.36336200000000002</v>
       </c>
       <c r="N346">
-        <v>0.84084150627241505</v>
+        <v>0.40371449702819301</v>
       </c>
       <c r="O346">
         <v>0</v>
@@ -18845,7 +18845,7 @@
         <v>0.39413100000000001</v>
       </c>
       <c r="N347">
-        <v>0.84084150627241505</v>
+        <v>0.544974066636152</v>
       </c>
       <c r="O347">
         <v>1</v>
@@ -18898,7 +18898,7 @@
         <v>0.53880099999999997</v>
       </c>
       <c r="N348">
-        <v>0.84084150627241505</v>
+        <v>0.84980719985513498</v>
       </c>
       <c r="O348">
         <v>-1</v>
@@ -18951,7 +18951,7 @@
         <v>0.39179900000000001</v>
       </c>
       <c r="N349">
-        <v>0.84084150627241505</v>
+        <v>0.874007879169865</v>
       </c>
       <c r="O349">
         <v>-1</v>
@@ -19004,7 +19004,7 @@
         <v>0.39404299999999998</v>
       </c>
       <c r="N350">
-        <v>0.84084150627241505</v>
+        <v>0.88083557938509005</v>
       </c>
       <c r="O350">
         <v>-1</v>
@@ -19057,7 +19057,7 @@
         <v>0.24838199999999999</v>
       </c>
       <c r="N351">
-        <v>0.84084150627241505</v>
+        <v>0.93184044991735904</v>
       </c>
       <c r="O351">
         <v>-1</v>
@@ -19110,7 +19110,7 @@
         <v>0.22522200000000001</v>
       </c>
       <c r="N352">
-        <v>0.84084150627241505</v>
+        <v>0.99684393353884704</v>
       </c>
       <c r="O352">
         <v>1</v>
@@ -19163,7 +19163,7 @@
         <v>0.29723699999999997</v>
       </c>
       <c r="N353">
-        <v>0.84084150627241505</v>
+        <v>0.40668766574878201</v>
       </c>
       <c r="O353">
         <v>1</v>
@@ -19216,7 +19216,7 @@
         <v>0.30010199999999998</v>
       </c>
       <c r="N354">
-        <v>0.84084150627241505</v>
+        <v>0.32623046974033298</v>
       </c>
       <c r="O354">
         <v>1</v>
@@ -19269,7 +19269,7 @@
         <v>0.44096000000000002</v>
       </c>
       <c r="N355">
-        <v>0.84084150627241505</v>
+        <v>0.36286705063439301</v>
       </c>
       <c r="O355">
         <v>0</v>
@@ -19290,7 +19290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99FDC657-1DEB-6D4A-8D22-B15F9273A3D1}">
   <dimension ref="A1:N355"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>

</xml_diff>